<commit_message>
CSV data reading fixes
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -37,13 +37,13 @@
     <t xml:space="preserve">probability</t>
   </si>
   <si>
-    <t xml:space="preserve">Итоговая вероятность</t>
+    <t xml:space="preserve">final_probability</t>
   </si>
   <si>
-    <t xml:space="preserve">Дисконтированная сумма</t>
+    <t xml:space="preserve">discount_sum</t>
   </si>
   <si>
-    <t xml:space="preserve">Итоговая дисконтированная сумма</t>
+    <t xml:space="preserve">final_discount_sum</t>
   </si>
   <si>
     <t xml:space="preserve">final_sum</t>
@@ -372,7 +372,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>